<commit_message>
update mb52 dari web
</commit_message>
<xml_diff>
--- a/data/mb52.xlsx
+++ b/data/mb52.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KAI\Data\MB52\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD85495C-8003-476F-A15B-0FE8E6445E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{24A0A94E-C1B8-4DD1-B413-58E736EADD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$1367</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$1366</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -5777,7 +5779,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -49507,8 +49509,32 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1367"/>
+  <autoFilter ref="A1:J1366"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>